<commit_message>
added more tables to the database design
</commit_message>
<xml_diff>
--- a/OnlineExamination-Class Diagram and DatabaseDesign.xlsx
+++ b/OnlineExamination-Class Diagram and DatabaseDesign.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Department</t>
   </si>
@@ -63,9 +63,6 @@
     <t>DCF_id</t>
   </si>
   <si>
-    <t>DCF_date</t>
-  </si>
-  <si>
     <t>(we could accept date and time &amp; split like Spring,Summer,Fall)</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>module_Id</t>
   </si>
   <si>
-    <t>module_name</t>
-  </si>
-  <si>
     <t>Department_Couse_Faculty_Date (Faculty Registration)</t>
   </si>
   <si>
@@ -133,13 +127,91 @@
   </si>
   <si>
     <t>fk_module_Id</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>DCSD</t>
+  </si>
+  <si>
+    <t>student_id</t>
+  </si>
+  <si>
+    <t>DCS_id</t>
+  </si>
+  <si>
+    <t>student_name</t>
+  </si>
+  <si>
+    <t>fk_student_id</t>
+  </si>
+  <si>
+    <t>student_email</t>
+  </si>
+  <si>
+    <t>student_phone No.</t>
+  </si>
+  <si>
+    <t>DCF_date_faculty</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>DCF_date_student</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Scheduler</t>
+  </si>
+  <si>
+    <t>Exam_names</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>schedule_id</t>
+  </si>
+  <si>
+    <t>exam_id</t>
+  </si>
+  <si>
+    <t>result_id</t>
+  </si>
+  <si>
+    <t>module_name(if module name is un assigned,we keep name as miscellaneous and update the module for that subject based on DCF_id)</t>
+  </si>
+  <si>
+    <t>Start_date and time</t>
+  </si>
+  <si>
+    <t>Exam_name</t>
+  </si>
+  <si>
+    <t>fk_exam_id</t>
+  </si>
+  <si>
+    <t>End_dtae and time</t>
+  </si>
+  <si>
+    <t>fk_DCS_id</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>(automatically trigger initiates and create a table in database for this subject questions)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +263,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -212,23 +291,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,180 +639,356 @@
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" ht="57" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="10"/>
+      <c r="B4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4"/>
-      <c r="B4" s="10" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="31.5">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="60">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="120">
+      <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="60">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="12" customHeight="1">
-      <c r="A9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57.75" customHeight="1">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="D12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="120">
+      <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>